<commit_message>
06: Excel data update
</commit_message>
<xml_diff>
--- a/06_MikrovlnInterfer/data/tloustka.xlsx
+++ b/06_MikrovlnInterfer/data/tloustka.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\PraktikumPlazma\06_MikrovlnInterfer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE2E44E-41A9-49CB-88BB-D4B8B38D5542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09EA4AC-AC79-4174-8858-15A168FCA3C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21000" yWindow="2715" windowWidth="7590" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3804" yWindow="3804" windowWidth="30960" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -460,18 +460,18 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.88671875" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -483,7 +483,7 @@
         <v>0.6108652381980153</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -491,7 +491,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -499,7 +499,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -508,7 +508,7 @@
         <v>149.93642442341445</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -517,7 +517,7 @@
         <v>38154.172727403726</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>0</v>
       </c>
@@ -526,7 +526,7 @@
         <v>21.063076015835875</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -539,13 +539,13 @@
         <v>2.4647398402715584E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9">
         <f>PI()*B2/4/SIN(C1)</f>
         <v>24.647398402715584</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -554,7 +554,7 @@
         <v>0.17199999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -575,7 +575,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -587,7 +587,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
06: Tex correction, vd data and graph, references
</commit_message>
<xml_diff>
--- a/06_MikrovlnInterfer/data/tloustka.xlsx
+++ b/06_MikrovlnInterfer/data/tloustka.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\PraktikumPlazma\06_MikrovlnInterfer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09EA4AC-AC79-4174-8858-15A168FCA3C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E8F87E-9EF8-4990-92A0-B75D998D82F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3804" yWindow="3804" windowWidth="30960" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>vyska/hloubka desky (prav.4bok) podobneho objemu [mm]</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>lambda_krit</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -457,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -471,7 +474,7 @@
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -483,7 +486,7 @@
         <v>0.6108652381980153</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -491,7 +494,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -499,7 +502,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -508,7 +511,7 @@
         <v>149.93642442341445</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -517,7 +520,7 @@
         <v>38154.172727403726</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>0</v>
       </c>
@@ -526,7 +529,7 @@
         <v>21.063076015835875</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -538,14 +541,18 @@
         <f>B8*0.001</f>
         <v>2.4647398402715584E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" s="2">
+        <f>PI()*B2^2/4/B3/SIN(C1)</f>
+        <v>5.1587578052195404</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9">
         <f>PI()*B2/4/SIN(C1)</f>
         <v>24.647398402715584</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -554,13 +561,22 @@
         <v>0.17199999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
       <c r="B11">
         <f>300000000/B10*0.000000001</f>
         <v>1.7441860465116283</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <f>PI()*(B2/1000)^2/4</f>
+        <v>2.5446900494077322E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
06: Plasma thickness and corresponding graphs correction
</commit_message>
<xml_diff>
--- a/06_MikrovlnInterfer/data/tloustka.xlsx
+++ b/06_MikrovlnInterfer/data/tloustka.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\PraktikumPlazma\06_MikrovlnInterfer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E8F87E-9EF8-4990-92A0-B75D998D82F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F8BABD-E94D-4A5E-9D0E-F9B463840367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3840" yWindow="3840" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>vyska/hloubka desky (prav.4bok) podobneho objemu [mm]</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>pricny rozmer vlnovodu a [mm]</t>
   </si>
 </sst>
 </file>
@@ -463,7 +466,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -496,10 +499,19 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <f>43</f>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -542,8 +554,8 @@
         <v>2.4647398402715584E-2</v>
       </c>
       <c r="D8" s="2">
-        <f>PI()*B2^2/4/B3/SIN(C1)</f>
-        <v>5.1587578052195404</v>
+        <f>PI()*B2^2/4/B4/SIN(C1)</f>
+        <v>10.317515610439081</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>